<commit_message>
bug fixes and cleanup
</commit_message>
<xml_diff>
--- a/Standardization/term_time_and_direction_switches.xlsx
+++ b/Standardization/term_time_and_direction_switches.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\Desktop\Master Project\wise-dag\Standardization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266E8861-89F9-4E50-87D8-278030496053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18C022A7-6E60-4648-891D-24225D761CD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1B1D6425-88FD-42FC-82B9-F7ED3685AD97}"/>
+    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{1B1D6425-88FD-42FC-82B9-F7ED3685AD97}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="312">
   <si>
     <t>term</t>
   </si>
@@ -1345,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247059F5-87D4-473B-B529-D3C8FC0596EF}">
   <dimension ref="A1:C309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A272" workbookViewId="0">
-      <selection activeCell="C295" sqref="C295"/>
+    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
+      <selection activeCell="J229" sqref="J229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2701,9 +2701,6 @@
       <c r="A253" t="s">
         <v>252</v>
       </c>
-      <c r="C253" t="s">
-        <v>311</v>
-      </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A254" t="s">

</xml_diff>